<commit_message>
Update portfolio analysis and remove old documentation
- Updated Portfolio_Analysis_3Sheets.xlsx with latest analysis
- Removed CORRELATION_UPDATE_SUMMARY.md (outdated)
- Removed FINAL_ANALYSIS_STATUS.txt (outdated)
</commit_message>
<xml_diff>
--- a/Portfolio_Analysis_3Sheets.xlsx
+++ b/Portfolio_Analysis_3Sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sureshpatil/Desktop/Portfolio Creation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A5E2DE-D1BA-3E45-BD8F-5C5D3365F7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4972513-1D21-5444-BF2B-A0C74FAD259E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3200" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3200" yWindow="-20980" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy_Statistics" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="199">
   <si>
     <t>FINAL PORTFOLIO ANALYSIS</t>
   </si>
@@ -630,15 +630,19 @@
   </si>
   <si>
     <t>Sharpe=(w×μ)/√(w×Σ×w), ρ=0.3</t>
+  </si>
+  <si>
+    <t>Alpha_T-stat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.00&quot;%&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -800,7 +804,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -915,8 +919,14 @@
         <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF3CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -954,11 +964,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -980,27 +999,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1020,28 +1035,55 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1344,103 +1386,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="17" width="14" customWidth="1"/>
+    <col min="2" max="18" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="5" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+    </row>
+    <row r="5" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -1492,8 +1535,11 @@
       <c r="Q6" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -1551,8 +1597,12 @@
       <c r="Q7" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7" s="46">
+        <f>B7*SQRT(C7)</f>
+        <v>17.874003468725185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>93</v>
       </c>
@@ -1610,8 +1660,12 @@
       <c r="Q8" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8" s="46">
+        <f>B8*SQRT(C8)</f>
+        <v>18.423639705552212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>95</v>
       </c>
@@ -1667,29 +1721,34 @@
         <f>SUM(Q7:Q8)</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="R9" s="54">
+        <f>B9*SQRT(C9)</f>
+        <v>25.710645655058915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
@@ -1741,8 +1800,11 @@
       <c r="Q13" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>97</v>
       </c>
@@ -1800,8 +1862,12 @@
       <c r="Q14" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14" s="9">
+        <f>B14*SQRT(C14)</f>
+        <v>29.225482031952868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>100</v>
       </c>
@@ -1859,8 +1925,12 @@
       <c r="Q15" s="2">
         <v>356</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15" s="9">
+        <f t="shared" ref="R15:R16" si="0">B15*SQRT(C15)</f>
+        <v>20.150558304920484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>95</v>
       </c>
@@ -1916,29 +1986,34 @@
         <f>SUM(Q14:Q15)</f>
         <v>386</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="R16" s="47">
+        <f t="shared" si="0"/>
+        <v>34.990391538249469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -1990,8 +2065,11 @@
       <c r="Q20" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R20" s="48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>103</v>
       </c>
@@ -2002,7 +2080,7 @@
         <v>301</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" ref="D21:D29" si="0">IF(C21&gt;0, (P21/C21)*100, 0)</f>
+        <f t="shared" ref="D21:D29" si="1">IF(C21&gt;0, (P21/C21)*100, 0)</f>
         <v>83.056478405315616</v>
       </c>
       <c r="E21" s="2">
@@ -2012,19 +2090,19 @@
         <v>778</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ref="G21:G28" si="1">F21*2</f>
+        <f t="shared" ref="G21:G28" si="2">F21*2</f>
         <v>1556</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21:H28" si="2">G21+E21</f>
+        <f t="shared" ref="H21:H28" si="3">G21+E21</f>
         <v>2920.46</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" ref="I21:I29" si="3">IF(G21&gt;0, (E21/G21)*100, 0)</f>
+        <f t="shared" ref="I21:I29" si="4">IF(G21&gt;0, (E21/G21)*100, 0)</f>
         <v>87.69023136246787</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" ref="J21:J28" si="4">IF(AND(G21&gt;0, M21&gt;0), ((1+I21/100)^(1/M21)-1)*100, 0)</f>
+        <f t="shared" ref="J21:J28" si="5">IF(AND(G21&gt;0, M21&gt;0), ((1+I21/100)^(1/M21)-1)*100, 0)</f>
         <v>12.995249585760194</v>
       </c>
       <c r="K21" s="2">
@@ -2034,7 +2112,7 @@
         <v>1881</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ref="M21:M28" si="5">L21/365</f>
+        <f t="shared" ref="M21:M28" si="6">L21/365</f>
         <v>5.1534246575342468</v>
       </c>
       <c r="N21" s="2" t="s">
@@ -2049,8 +2127,12 @@
       <c r="Q21" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R21" s="49">
+        <f>B21*SQRT(C21)</f>
+        <v>91.778069820627621</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>106</v>
       </c>
@@ -2061,7 +2143,7 @@
         <v>124</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81.451612903225808</v>
       </c>
       <c r="E22" s="2">
@@ -2071,19 +2153,19 @@
         <v>408.1</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>816.2</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1430.69</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.286694437637834</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.656482853874728</v>
       </c>
       <c r="K22" s="2">
@@ -2093,7 +2175,7 @@
         <v>1858</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0904109589041093</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -2108,8 +2190,12 @@
       <c r="Q22" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22" s="49">
+        <f t="shared" ref="R22:R29" si="7">B22*SQRT(C22)</f>
+        <v>31.17948043184812</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>109</v>
       </c>
@@ -2120,7 +2206,7 @@
         <v>109</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82.568807339449549</v>
       </c>
       <c r="E23" s="2">
@@ -2130,19 +2216,19 @@
         <v>154.80000000000001</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>309.60000000000002</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>757.17000000000007</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>144.56395348837208</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.733421849156649</v>
       </c>
       <c r="K23" s="2">
@@ -2152,7 +2238,7 @@
         <v>1901</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.2082191780821914</v>
       </c>
       <c r="N23" s="2" t="s">
@@ -2167,8 +2253,12 @@
       <c r="Q23" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23" s="49">
+        <f t="shared" si="7"/>
+        <v>37.167491171721558</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>111</v>
       </c>
@@ -2179,7 +2269,7 @@
         <v>106</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>87.735849056603783</v>
       </c>
       <c r="E24" s="2">
@@ -2189,19 +2279,19 @@
         <v>93.2</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>186.4</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>605.13</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>224.64055793991417</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.042801356891143</v>
       </c>
       <c r="K24" s="2">
@@ -2211,7 +2301,7 @@
         <v>1857</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.087671232876712</v>
       </c>
       <c r="N24" s="2" t="s">
@@ -2226,8 +2316,12 @@
       <c r="Q24" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24" s="49">
+        <f t="shared" si="7"/>
+        <v>46.53624823726124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>114</v>
       </c>
@@ -2238,7 +2332,7 @@
         <v>132</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81.818181818181827</v>
       </c>
       <c r="E25" s="2">
@@ -2248,19 +2342,19 @@
         <v>289.60000000000002</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>579.20000000000005</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>958.51</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65.488604972375683</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.8664454967939861</v>
       </c>
       <c r="K25" s="2">
@@ -2270,7 +2364,7 @@
         <v>1954</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.353424657534247</v>
       </c>
       <c r="N25" s="2" t="s">
@@ -2285,8 +2379,12 @@
       <c r="Q25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25" s="49">
+        <f t="shared" si="7"/>
+        <v>37.569439708358708</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>117</v>
       </c>
@@ -2297,7 +2395,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>88.495575221238937</v>
       </c>
       <c r="E26" s="2">
@@ -2307,19 +2405,19 @@
         <v>116.2</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>232.4</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>785.12</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>237.8313253012048</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.281152365685202</v>
       </c>
       <c r="K26" s="2">
@@ -2329,7 +2427,7 @@
         <v>1842</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0465753424657533</v>
       </c>
       <c r="N26" s="2" t="s">
@@ -2344,8 +2442,12 @@
       <c r="Q26" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26" s="49">
+        <f t="shared" si="7"/>
+        <v>55.914566974984254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>119</v>
       </c>
@@ -2356,7 +2458,7 @@
         <v>265</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86.79245283018868</v>
       </c>
       <c r="E27" s="2">
@@ -2366,19 +2468,19 @@
         <v>356.6</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>713.2</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1713.6100000000001</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140.2706113292204</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.557576988067993</v>
       </c>
       <c r="K27" s="2">
@@ -2388,7 +2490,7 @@
         <v>1978</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.419178082191781</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -2403,8 +2505,12 @@
       <c r="Q27" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27" s="49">
+        <f t="shared" si="7"/>
+        <v>117.37029649787888</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>122</v>
       </c>
@@ -2415,7 +2521,7 @@
         <v>669</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.109118086696569</v>
       </c>
       <c r="E28" s="2">
@@ -2425,19 +2531,19 @@
         <v>459.6</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>919.2</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2731.98</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>197.21279373368145</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22.375386638341421</v>
       </c>
       <c r="K28" s="2">
@@ -2447,7 +2553,7 @@
         <v>1969</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.3945205479452056</v>
       </c>
       <c r="N28" s="2" t="s">
@@ -2462,8 +2568,12 @@
       <c r="Q28" s="2">
         <v>113</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28" s="49">
+        <f t="shared" si="7"/>
+        <v>201.22996695323488</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -2476,7 +2586,7 @@
         <v>1819</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.002199010445295</v>
       </c>
       <c r="E29" s="3">
@@ -2496,7 +2606,7 @@
         <v>11902.67</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124.06291178795979</v>
       </c>
       <c r="J29" s="3">
@@ -2519,29 +2629,34 @@
         <f>SUM(Q21:Q28)</f>
         <v>291</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="38" t="s">
+      <c r="R29" s="55">
+        <f t="shared" si="7"/>
+        <v>211.59600384267071</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="52"/>
+      <c r="R32" s="52"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -2593,8 +2708,11 @@
       <c r="Q33" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>126</v>
       </c>
@@ -2605,7 +2723,7 @@
         <v>400</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:D40" si="6">IF(C34&gt;0, (P34/C34)*100, 0)</f>
+        <f t="shared" ref="D34:D40" si="8">IF(C34&gt;0, (P34/C34)*100, 0)</f>
         <v>66.5</v>
       </c>
       <c r="E34" s="2">
@@ -2615,19 +2733,19 @@
         <v>19.28</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ref="G34:G39" si="7">F34*2</f>
+        <f t="shared" ref="G34:G39" si="9">F34*2</f>
         <v>38.56</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" ref="H34:H39" si="8">G34+E34</f>
+        <f t="shared" ref="H34:H39" si="10">G34+E34</f>
         <v>79.53</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" ref="I34:I40" si="9">IF(G34&gt;0, (E34/G34)*100, 0)</f>
+        <f t="shared" ref="I34:I40" si="11">IF(G34&gt;0, (E34/G34)*100, 0)</f>
         <v>106.25</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J39" si="10">IF(AND(G34&gt;0, M34&gt;0), ((1+I34/100)^(1/M34)-1)*100, 0)</f>
+        <f t="shared" ref="J34:J39" si="12">IF(AND(G34&gt;0, M34&gt;0), ((1+I34/100)^(1/M34)-1)*100, 0)</f>
         <v>12.993398690782465</v>
       </c>
       <c r="K34" s="2">
@@ -2637,7 +2755,7 @@
         <v>2163</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34:M39" si="11">L34/365</f>
+        <f t="shared" ref="M34:M39" si="13">L34/365</f>
         <v>5.9260273972602739</v>
       </c>
       <c r="N34" s="2" t="s">
@@ -2652,8 +2770,12 @@
       <c r="Q34" s="2">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34" s="49">
+        <f>B34*SQRT(C34)</f>
+        <v>28.799999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>129</v>
       </c>
@@ -2664,7 +2786,7 @@
         <v>354</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>62.711864406779661</v>
       </c>
       <c r="E35" s="2">
@@ -2674,19 +2796,19 @@
         <v>23.23</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>46.46</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>81.050000000000011</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.451140766250546</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.8692721491212119</v>
       </c>
       <c r="K35" s="2">
@@ -2696,7 +2818,7 @@
         <v>2158</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.912328767123288</v>
       </c>
       <c r="N35" s="2" t="s">
@@ -2711,8 +2833,12 @@
       <c r="Q35" s="2">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35" s="49">
+        <f t="shared" ref="R35:R40" si="14">B35*SQRT(C35)</f>
+        <v>15.804505686670494</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>131</v>
       </c>
@@ -2723,7 +2849,7 @@
         <v>301</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>58.471760797342199</v>
       </c>
       <c r="E36" s="2">
@@ -2733,19 +2859,19 @@
         <v>17.09</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>34.18</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>55.54</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>62.492685781158578</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8.4434355217986035</v>
       </c>
       <c r="K36" s="2">
@@ -2755,7 +2881,7 @@
         <v>2186</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9890410958904106</v>
       </c>
       <c r="N36" s="2" t="s">
@@ -2770,8 +2896,12 @@
       <c r="Q36" s="2">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36" s="49">
+        <f t="shared" si="14"/>
+        <v>15.614416415607725</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>133</v>
       </c>
@@ -2782,7 +2912,7 @@
         <v>192</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>65.625</v>
       </c>
       <c r="E37" s="2">
@@ -2792,19 +2922,19 @@
         <v>20.25</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>40.5</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>59.39</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>46.641975308641975</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.8869842175339535</v>
       </c>
       <c r="K37" s="2">
@@ -2814,7 +2944,7 @@
         <v>2098</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.7479452054794518</v>
       </c>
       <c r="N37" s="2" t="s">
@@ -2829,8 +2959,12 @@
       <c r="Q37" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37" s="49">
+        <f t="shared" si="14"/>
+        <v>13.163586137523467</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>135</v>
       </c>
@@ -2841,7 +2975,7 @@
         <v>218</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>62.844036697247709</v>
       </c>
       <c r="E38" s="2">
@@ -2851,19 +2985,19 @@
         <v>16.829999999999998</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>33.659999999999997</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>58.03</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>72.400475341651827</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.6264072782966004</v>
       </c>
       <c r="K38" s="2">
@@ -2873,7 +3007,7 @@
         <v>2163</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9260273972602739</v>
       </c>
       <c r="N38" s="2" t="s">
@@ -2888,8 +3022,12 @@
       <c r="Q38" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R38" s="49">
+        <f t="shared" si="14"/>
+        <v>12.55009960119839</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>136</v>
       </c>
@@ -2900,7 +3038,7 @@
         <v>258</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>64.341085271317837</v>
       </c>
       <c r="E39" s="2">
@@ -2910,19 +3048,19 @@
         <v>6.34</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12.68</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>36.739999999999995</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>189.74763406940062</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>19.644434183936998</v>
       </c>
       <c r="K39" s="2">
@@ -2932,7 +3070,7 @@
         <v>2165</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9315068493150687</v>
       </c>
       <c r="N39" s="2" t="s">
@@ -2947,8 +3085,12 @@
       <c r="Q39" s="2">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R39" s="49">
+        <f t="shared" si="14"/>
+        <v>14.456140563788109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>95</v>
       </c>
@@ -2961,7 +3103,7 @@
         <v>1723</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>63.43586767266396</v>
       </c>
       <c r="E40" s="3">
@@ -2981,7 +3123,7 @@
         <v>370.28</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>79.712677150067947</v>
       </c>
       <c r="J40" s="3">
@@ -3004,29 +3146,34 @@
         <f>SUM(Q34:Q39)</f>
         <v>630</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="33" t="s">
+      <c r="R40" s="55">
+        <f t="shared" si="14"/>
+        <v>40.678854457813827</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="27"/>
+      <c r="R43" s="27"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>75</v>
       </c>
@@ -3078,8 +3225,11 @@
       <c r="Q44" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R44" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>139</v>
       </c>
@@ -3090,7 +3240,7 @@
         <v>234</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" ref="D45:D60" si="12">IF(C45&gt;0, (P45/C45)*100, 0)</f>
+        <f t="shared" ref="D45:D60" si="15">IF(C45&gt;0, (P45/C45)*100, 0)</f>
         <v>74.358974358974365</v>
       </c>
       <c r="E45" s="2">
@@ -3100,19 +3250,19 @@
         <v>323.61</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" ref="G45:G59" si="13">F45*2</f>
+        <f t="shared" ref="G45:G59" si="16">F45*2</f>
         <v>647.22</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" ref="H45:H59" si="14">G45+E45</f>
+        <f t="shared" ref="H45:H59" si="17">G45+E45</f>
         <v>1122.51</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" ref="I45:I60" si="15">IF(G45&gt;0, (E45/G45)*100, 0)</f>
+        <f t="shared" ref="I45:I60" si="18">IF(G45&gt;0, (E45/G45)*100, 0)</f>
         <v>73.435616946324274</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" ref="J45:J59" si="16">IF(AND(G45&gt;0, M45&gt;0), ((1+I45/100)^(1/M45)-1)*100, 0)</f>
+        <f t="shared" ref="J45:J59" si="19">IF(AND(G45&gt;0, M45&gt;0), ((1+I45/100)^(1/M45)-1)*100, 0)</f>
         <v>10.144843704482675</v>
       </c>
       <c r="K45" s="2">
@@ -3122,7 +3272,7 @@
         <v>2080</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" ref="M45:M59" si="17">L45/365</f>
+        <f t="shared" ref="M45:M59" si="20">L45/365</f>
         <v>5.6986301369863011</v>
       </c>
       <c r="N45" s="2" t="s">
@@ -3137,8 +3287,12 @@
       <c r="Q45" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R45" s="49">
+        <f>B45*SQRT(C45)</f>
+        <v>39.925322791431505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>103</v>
       </c>
@@ -3149,7 +3303,7 @@
         <v>235</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>71.914893617021278</v>
       </c>
       <c r="E46" s="2">
@@ -3159,19 +3313,19 @@
         <v>1262.53</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2525.06</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3025.69</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>19.826459569277564</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.2264812318246738</v>
       </c>
       <c r="K46" s="2">
@@ -3181,7 +3335,7 @@
         <v>2079</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.6958904109589037</v>
       </c>
       <c r="N46" s="2" t="s">
@@ -3196,8 +3350,12 @@
       <c r="Q46" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R46" s="49">
+        <f t="shared" ref="R46:R60" si="21">B46*SQRT(C46)</f>
+        <v>15.483006813923451</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>106</v>
       </c>
@@ -3208,7 +3366,7 @@
         <v>228</v>
       </c>
       <c r="D47" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>72.368421052631575</v>
       </c>
       <c r="E47" s="2">
@@ -3218,19 +3376,19 @@
         <v>735.54</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1471.08</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1933</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>31.400059819996194</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.0122896559965602</v>
       </c>
       <c r="K47" s="2">
@@ -3240,7 +3398,7 @@
         <v>2038</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.5835616438356164</v>
       </c>
       <c r="N47" s="2" t="s">
@@ -3255,8 +3413,12 @@
       <c r="Q47" s="2">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R47" s="49">
+        <f t="shared" si="21"/>
+        <v>21.139536418758098</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>143</v>
       </c>
@@ -3267,7 +3429,7 @@
         <v>128</v>
       </c>
       <c r="D48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75.78125</v>
       </c>
       <c r="E48" s="2">
@@ -3277,19 +3439,19 @@
         <v>727.1</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1454.2</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1722.1100000000001</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>18.423188007151701</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.0808942620801583</v>
       </c>
       <c r="K48" s="2">
@@ -3299,7 +3461,7 @@
         <v>2034</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.5726027397260278</v>
       </c>
       <c r="N48" s="2" t="s">
@@ -3314,8 +3476,12 @@
       <c r="Q48" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48" s="49">
+        <f t="shared" si="21"/>
+        <v>11.426845583974609</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>145</v>
       </c>
@@ -3326,7 +3492,7 @@
         <v>230</v>
       </c>
       <c r="D49" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>73.043478260869563</v>
       </c>
       <c r="E49" s="2">
@@ -3336,19 +3502,19 @@
         <v>317.39999999999998</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>634.79999999999995</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1007.1399999999999</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>58.65469439193447</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>8.5434349837455024</v>
       </c>
       <c r="K49" s="2">
@@ -3358,7 +3524,7 @@
         <v>2055</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.6301369863013697</v>
       </c>
       <c r="N49" s="2" t="s">
@@ -3373,8 +3539,12 @@
       <c r="Q49" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R49" s="49">
+        <f t="shared" si="21"/>
+        <v>33.061336936064762</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -3385,7 +3555,7 @@
         <v>188</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>69.148936170212778</v>
       </c>
       <c r="E50" s="2">
@@ -3395,19 +3565,19 @@
         <v>486.55</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>973.1</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1227.7</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>26.163806391943272</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.3305248701648758</v>
       </c>
       <c r="K50" s="2">
@@ -3417,7 +3587,7 @@
         <v>2001</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.4821917808219176</v>
       </c>
       <c r="N50" s="2" t="s">
@@ -3432,8 +3602,12 @@
       <c r="Q50" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R50" s="49">
+        <f t="shared" si="21"/>
+        <v>14.945327028874276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>109</v>
       </c>
@@ -3444,7 +3618,7 @@
         <v>249</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>73.493975903614455</v>
       </c>
       <c r="E51" s="2">
@@ -3454,19 +3628,19 @@
         <v>141.11000000000001</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>282.22000000000003</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>691.75</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>145.11019771809225</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>17.417685409072071</v>
       </c>
       <c r="K51" s="2">
@@ -3476,7 +3650,7 @@
         <v>2038</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.5835616438356164</v>
       </c>
       <c r="N51" s="2" t="s">
@@ -3491,8 +3665,12 @@
       <c r="Q51" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R51" s="49">
+        <f t="shared" si="21"/>
+        <v>49.390566913126229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>149</v>
       </c>
@@ -3503,7 +3681,7 @@
         <v>270</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>71.851851851851862</v>
       </c>
       <c r="E52" s="2">
@@ -3513,19 +3691,19 @@
         <v>495.84</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>991.68</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1325.85</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>33.697362052274933</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.4095931737067726</v>
       </c>
       <c r="K52" s="2">
@@ -3535,7 +3713,7 @@
         <v>2012</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.5123287671232877</v>
       </c>
       <c r="N52" s="2" t="s">
@@ -3550,8 +3728,12 @@
       <c r="Q52" s="2">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R52" s="49">
+        <f t="shared" si="21"/>
+        <v>23.990248018726273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>151</v>
       </c>
@@ -3562,7 +3744,7 @@
         <v>179</v>
       </c>
       <c r="D53" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>72.067039106145245</v>
       </c>
       <c r="E53" s="2">
@@ -3572,19 +3754,19 @@
         <v>592.92999999999995</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1185.8599999999999</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1425.7099999999998</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>20.225827669370751</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.3208898889682592</v>
       </c>
       <c r="K53" s="2">
@@ -3594,7 +3776,7 @@
         <v>2058</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.6383561643835618</v>
       </c>
       <c r="N53" s="2" t="s">
@@ -3609,8 +3791,12 @@
       <c r="Q53" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R53" s="49">
+        <f t="shared" si="21"/>
+        <v>17.259023726734952</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>153</v>
       </c>
@@ -3621,7 +3807,7 @@
         <v>323</v>
       </c>
       <c r="D54" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>69.040247678018574</v>
       </c>
       <c r="E54" s="2">
@@ -3631,19 +3817,19 @@
         <v>674.92</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1349.84</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1656.1</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>22.68861494695668</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.7620098074273134</v>
       </c>
       <c r="K54" s="2">
@@ -3653,7 +3839,7 @@
         <v>2021</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.536986301369863</v>
       </c>
       <c r="N54" s="2" t="s">
@@ -3668,8 +3854,12 @@
       <c r="Q54" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R54" s="49">
+        <f t="shared" si="21"/>
+        <v>17.433034732943085</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3680,7 +3870,7 @@
         <v>250</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75.599999999999994</v>
       </c>
       <c r="E55" s="2">
@@ -3690,19 +3880,19 @@
         <v>553.53</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1107.06</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1455.83</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>31.504164182609795</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.1015735577188748</v>
       </c>
       <c r="K55" s="2">
@@ -3712,7 +3902,7 @@
         <v>2009</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.5041095890410956</v>
       </c>
       <c r="N55" s="2" t="s">
@@ -3727,8 +3917,12 @@
       <c r="Q55" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R55" s="49">
+        <f t="shared" si="21"/>
+        <v>24.191424100288103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>157</v>
       </c>
@@ -3739,7 +3933,7 @@
         <v>224</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>73.214285714285708</v>
       </c>
       <c r="E56" s="2">
@@ -3749,19 +3943,19 @@
         <v>763.98</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1527.96</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>2168.7600000000002</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>41.938270635356943</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.5294606769438657</v>
       </c>
       <c r="K56" s="2">
@@ -3771,7 +3965,7 @@
         <v>2021</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.536986301369863</v>
       </c>
       <c r="N56" s="2" t="s">
@@ -3786,8 +3980,12 @@
       <c r="Q56" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R56" s="49">
+        <f t="shared" si="21"/>
+        <v>22.898943207056522</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>117</v>
       </c>
@@ -3798,7 +3996,7 @@
         <v>205</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>67.804878048780495</v>
       </c>
       <c r="E57" s="2">
@@ -3808,19 +4006,19 @@
         <v>267.04000000000002</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>534.08000000000004</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>794.17000000000007</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>48.698696824445769</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>7.8214598428950177</v>
       </c>
       <c r="K57" s="2">
@@ -3830,7 +4028,7 @@
         <v>1923</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.2684931506849315</v>
       </c>
       <c r="N57" s="2" t="s">
@@ -3845,8 +4043,12 @@
       <c r="Q57" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R57" s="49">
+        <f t="shared" si="21"/>
+        <v>26.487968967061256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>119</v>
       </c>
@@ -3857,7 +4059,7 @@
         <v>257</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>73.540856031128413</v>
       </c>
       <c r="E58" s="2">
@@ -3867,19 +4069,19 @@
         <v>256.2</v>
       </c>
       <c r="G58" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>512.4</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>844.69</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>64.849726775956299</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>9.5917124455183966</v>
       </c>
       <c r="K58" s="2">
@@ -3889,7 +4091,7 @@
         <v>1992</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.4575342465753423</v>
       </c>
       <c r="N58" s="2" t="s">
@@ -3904,8 +4106,12 @@
       <c r="Q58" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R58" s="49">
+        <f t="shared" si="21"/>
+        <v>34.787746405882636</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>122</v>
       </c>
@@ -3916,7 +4122,7 @@
         <v>192</v>
       </c>
       <c r="D59" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>77.083333333333343</v>
       </c>
       <c r="E59" s="2">
@@ -3926,19 +4132,19 @@
         <v>149.09</v>
       </c>
       <c r="G59" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>298.18</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>555.25</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>86.213025689181023</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>12.525242819703442</v>
       </c>
       <c r="K59" s="2">
@@ -3948,7 +4154,7 @@
         <v>1923</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.2684931506849315</v>
       </c>
       <c r="N59" s="2" t="s">
@@ -3963,8 +4169,12 @@
       <c r="Q59" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R59" s="49">
+        <f t="shared" si="21"/>
+        <v>59.028291521947331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>95</v>
       </c>
@@ -3977,7 +4187,7 @@
         <v>3392</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>72.553066037735846</v>
       </c>
       <c r="E60" s="3">
@@ -3997,7 +4207,7 @@
         <v>20956.259999999998</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>35.247574338130221</v>
       </c>
       <c r="J60" s="3">
@@ -4020,29 +4230,34 @@
         <f>SUM(Q45:Q59)</f>
         <v>931</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="36" t="s">
+      <c r="R60" s="55">
+        <f t="shared" si="21"/>
+        <v>106.73611779003811</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
+      <c r="L63" s="53"/>
+      <c r="M63" s="53"/>
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="Q63" s="53"/>
+      <c r="R63" s="53"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>75</v>
       </c>
@@ -4094,8 +4309,11 @@
       <c r="Q64" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R64" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>161</v>
       </c>
@@ -4153,8 +4371,12 @@
       <c r="Q65" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R65" s="49">
+        <f>B65*SQRT(C65)</f>
+        <v>72.580989246496216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>162</v>
       </c>
@@ -4212,8 +4434,12 @@
       <c r="Q66" s="2">
         <v>229</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R66" s="49">
+        <f t="shared" ref="R66:R67" si="22">B66*SQRT(C66)</f>
+        <v>204.89594163867665</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>95</v>
       </c>
@@ -4269,29 +4495,34 @@
         <f>SUM(Q65:Q66)</f>
         <v>233</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="30" t="s">
+      <c r="R67" s="49">
+        <f t="shared" si="22"/>
+        <v>197.25702535017604</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
-      <c r="K70" s="18"/>
-      <c r="L70" s="18"/>
-      <c r="M70" s="18"/>
-      <c r="N70" s="18"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="18"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -4343,8 +4574,11 @@
       <c r="Q71" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R71" s="48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>164</v>
       </c>
@@ -4355,7 +4589,7 @@
         <v>60</v>
       </c>
       <c r="D72" s="2">
-        <f t="shared" ref="D72:D77" si="18">IF(C72&gt;0, (P72/C72)*100, 0)</f>
+        <f t="shared" ref="D72:D77" si="23">IF(C72&gt;0, (P72/C72)*100, 0)</f>
         <v>61.666666666666671</v>
       </c>
       <c r="E72" s="2">
@@ -4373,7 +4607,7 @@
         <v>3114.23</v>
       </c>
       <c r="I72" s="2">
-        <f t="shared" ref="I72:I77" si="19">IF(G72&gt;0, (E72/G72)*100, 0)</f>
+        <f t="shared" ref="I72:I77" si="24">IF(G72&gt;0, (E72/G72)*100, 0)</f>
         <v>120.86737588652483</v>
       </c>
       <c r="J72" s="2">
@@ -4402,8 +4636,12 @@
       <c r="Q72" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R72" s="46">
+        <f>B72*SQRT(C72)</f>
+        <v>10.147216367063432</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>131</v>
       </c>
@@ -4414,7 +4652,7 @@
         <v>173</v>
       </c>
       <c r="D73" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>60.693641618497111</v>
       </c>
       <c r="E73" s="2">
@@ -4432,7 +4670,7 @@
         <v>8426.1</v>
       </c>
       <c r="I73" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>136.82124789207421</v>
       </c>
       <c r="J73" s="2">
@@ -4461,8 +4699,12 @@
       <c r="Q73" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R73" s="46">
+        <f t="shared" ref="R73:R77" si="25">B73*SQRT(C73)</f>
+        <v>11.04847500789136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>166</v>
       </c>
@@ -4473,7 +4715,7 @@
         <v>148</v>
       </c>
       <c r="D74" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>58.108108108108105</v>
       </c>
       <c r="E74" s="2">
@@ -4491,7 +4733,7 @@
         <v>6930.32</v>
       </c>
       <c r="I74" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>71.542574257425755</v>
       </c>
       <c r="J74" s="2">
@@ -4520,8 +4762,12 @@
       <c r="Q74" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R74" s="46">
+        <f t="shared" si="25"/>
+        <v>6.9343492845399695</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>168</v>
       </c>
@@ -4532,7 +4778,7 @@
         <v>400</v>
       </c>
       <c r="D75" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>60.25</v>
       </c>
       <c r="E75" s="2">
@@ -4550,7 +4796,7 @@
         <v>17800.650000000001</v>
       </c>
       <c r="I75" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>147.50625695216908</v>
       </c>
       <c r="J75" s="2">
@@ -4579,8 +4825,12 @@
       <c r="Q75" s="2">
         <v>159</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R75" s="46">
+        <f t="shared" si="25"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>136</v>
       </c>
@@ -4591,7 +4841,7 @@
         <v>622</v>
       </c>
       <c r="D76" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>62.861736334405151</v>
       </c>
       <c r="E76" s="2">
@@ -4609,7 +4859,7 @@
         <v>25515.46</v>
       </c>
       <c r="I76" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>178.61388949552304</v>
       </c>
       <c r="J76" s="2">
@@ -4638,8 +4888,12 @@
       <c r="Q76" s="2">
         <v>231</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R76" s="46">
+        <f t="shared" si="25"/>
+        <v>21.198938652677874</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>95</v>
       </c>
@@ -4652,7 +4906,7 @@
         <v>1403</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>61.297220242337843</v>
       </c>
       <c r="E77" s="3">
@@ -4672,7 +4926,7 @@
         <v>61786.76</v>
       </c>
       <c r="I77" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>143.65785945263821</v>
       </c>
       <c r="J77" s="3">
@@ -4695,19 +4949,23 @@
         <f>SUM(Q72:Q76)</f>
         <v>543</v>
       </c>
+      <c r="R77" s="54">
+        <f t="shared" si="25"/>
+        <v>32.437451626168162</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A63:R63"/>
+    <mergeCell ref="A70:R70"/>
     <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A32:Q32"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="A70:Q70"/>
     <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A12:Q12"/>
-    <mergeCell ref="A43:Q43"/>
     <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A19:Q19"/>
-    <mergeCell ref="A63:Q63"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="A12:R12"/>
+    <mergeCell ref="A19:R19"/>
+    <mergeCell ref="A32:R32"/>
+    <mergeCell ref="A43:R43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4717,8 +4975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4728,52 +4986,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -4941,124 +5199,124 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="18">
         <f t="array" ref="B12">SUMPRODUCT(B6:B7/100, G6:G7*J6:J7)/SQRT((1-0.3)*SUMPRODUCT((B6:B7/100)^2, J6:J7^2) + 0.3*(SUMPRODUCT(B6:B7/100, J6:J7))^2)</f>
         <v>1.8193702407364141</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="18">
         <f>SUMPRODUCT(B6:B7/100, I6:I7)</f>
         <v>19.238700905829099</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="18">
         <f>SUMPRODUCT(C6:C7/100, G6:G7*J6:J7)/SQRT((1-0.3)*SUMPRODUCT((C6:C7/100)^2, J6:J7^2) + 0.3*(SUMPRODUCT(C6:C7/100, J6:J7))^2)</f>
         <v>1.8171030484550312</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="18">
         <f>SUMPRODUCT(C6:C7/100, I6:I7)</f>
         <v>19.376449181386313</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14" s="18">
         <f>SUMPRODUCT(D6:D7/100, G6:G7*J6:J7)/SQRT((1-0.3)*SUMPRODUCT((D6:D7/100)^2, J6:J7^2) + 0.3*(SUMPRODUCT(D6:D7/100, J6:J7))^2)</f>
         <v>1.816517957182191</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="18">
         <f>SUMPRODUCT(D6:D7/100, I6:I7)</f>
         <v>19.191363263145348</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="18">
         <f>SUMPRODUCT(E6:E7/100, G6:G7*J6:J7)/SQRT((1-0.3)*SUMPRODUCT((E6:E7/100)^2, J6:J7^2) + 0.3*(SUMPRODUCT(E6:E7/100, J6:J7))^2)</f>
         <v>1.8197236017673823</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="18">
         <f>SUMPRODUCT(E6:E7/100, I6:I7)</f>
         <v>19.329538003951967</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="18">
         <f>SUMPRODUCT(F6:F7/100, G6:G7*J6:J7)/SQRT((1-0.3)*SUMPRODUCT((F6:F7/100)^2, J6:J7^2) + 0.3*(SUMPRODUCT(F6:F7/100, J6:J7))^2)</f>
         <v>1.817726538201847</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="18">
         <f>SUMPRODUCT(F6:F7/100, I6:I7)</f>
         <v>19.367919876398247</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -5226,124 +5484,124 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="18">
         <f>SUMPRODUCT(B21:B22/100, G21:G22*J21:J22)/SQRT((1-0.3)*SUMPRODUCT((B21:B22/100)^2, J21:J22^2) + 0.3*(SUMPRODUCT(B21:B22/100, J21:J22))^2)</f>
         <v>1.0190831141736116</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="18">
         <f>SUMPRODUCT(B21:B22/100, I21:I22)</f>
         <v>20.762847362954027</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="18">
         <f>SUMPRODUCT(C21:C22/100, G21:G22*J21:J22)/SQRT((1-0.3)*SUMPRODUCT((C21:C22/100)^2, J21:J22^2) + 0.3*(SUMPRODUCT(C21:C22/100, J21:J22))^2)</f>
         <v>1.3085323620205398</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="18">
         <f>SUMPRODUCT(C21:C22/100, I21:I22)</f>
         <v>22.39809888444465</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="18">
         <f>SUMPRODUCT(D21:D22/100, G21:G22*J21:J22)/SQRT((1-0.3)*SUMPRODUCT((D21:D22/100)^2, J21:J22^2) + 0.3*(SUMPRODUCT(D21:D22/100, J21:J22))^2)</f>
         <v>1.0824908754409048</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="18">
         <f>SUMPRODUCT(D21:D22/100, I21:I22)</f>
         <v>21.234218797974457</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="18">
         <f>SUMPRODUCT(E21:E22/100, G21:G22*J21:J22)/SQRT((1-0.3)*SUMPRODUCT((E21:E22/100)^2, J21:J22^2) + 0.3*(SUMPRODUCT(E21:E22/100, J21:J22))^2)</f>
         <v>1.1634689230500281</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="18">
         <f>SUMPRODUCT(E21:E22/100, I21:I22)</f>
         <v>21.702680532778711</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="18">
         <f>SUMPRODUCT(F21:F22/100, G21:G22*J21:J22)/SQRT((1-0.3)*SUMPRODUCT((F21:F22/100)^2, J21:J22^2) + 0.3*(SUMPRODUCT(F21:F22/100, J21:J22))^2)</f>
         <v>1.3531045130933623</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="18">
         <f>SUMPRODUCT(F21:F22/100, I21:I22)</f>
         <v>22.745323110241589</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -5763,124 +6021,124 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="44" t="s">
+      <c r="C47" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="43">
+      <c r="B48" s="18">
         <f>SUMPRODUCT(B36:B43/100, G36:G43*J36:J43)/SQRT((1-0.3)*SUMPRODUCT((B36:B43/100)^2, J36:J43^2) + 0.3*(SUMPRODUCT(B36:B43/100, J36:J43))^2)</f>
         <v>8.0664273247076395</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="18">
         <f>SUMPRODUCT(B36:B43/100, I36:I43)</f>
         <v>18.31357015240323</v>
       </c>
-      <c r="D48" s="43" t="s">
+      <c r="D48" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="43">
+      <c r="B49" s="18">
         <f>SUMPRODUCT(C36:C43/100, G36:G43*J36:J43)/SQRT((1-0.3)*SUMPRODUCT((C36:C43/100)^2, J36:J43^2) + 0.3*(SUMPRODUCT(C36:C43/100, J36:J43))^2)</f>
         <v>7.9701927644745192</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="18">
         <f>SUMPRODUCT(C36:C43/100, I36:I43)</f>
         <v>21.402554042665098</v>
       </c>
-      <c r="D49" s="43" t="s">
+      <c r="D49" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="43">
+      <c r="B50" s="18">
         <f>SUMPRODUCT(D36:D43/100, G36:G43*J36:J43)/SQRT((1-0.3)*SUMPRODUCT((D36:D43/100)^2, J36:J43^2) + 0.3*(SUMPRODUCT(D36:D43/100, J36:J43))^2)</f>
         <v>8.7974764430177714</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="18">
         <f>SUMPRODUCT(D36:D43/100, I36:I43)</f>
         <v>19.204257283993392</v>
       </c>
-      <c r="D50" s="43" t="s">
+      <c r="D50" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="43">
+      <c r="B51" s="18">
         <f>SUMPRODUCT(E36:E43/100, G36:G43*J36:J43)/SQRT((1-0.3)*SUMPRODUCT((E36:E43/100)^2, J36:J43^2) + 0.3*(SUMPRODUCT(E36:E43/100, J36:J43))^2)</f>
         <v>8.7813611382999532</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="18">
         <f>SUMPRODUCT(E36:E43/100, I36:I43)</f>
         <v>22.038848091221066</v>
       </c>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="43">
+      <c r="B52" s="18">
         <f>SUMPRODUCT(F36:F43/100, G36:G43*J36:J43)/SQRT((1-0.3)*SUMPRODUCT((F36:F43/100)^2, J36:J43^2) + 0.3*(SUMPRODUCT(F36:F43/100, J36:J43))^2)</f>
         <v>8.9466043896702931</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="18">
         <f>SUMPRODUCT(F36:F43/100, I36:I43)</f>
         <v>23.785295460758309</v>
       </c>
-      <c r="D52" s="43" t="s">
+      <c r="D52" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
@@ -6216,124 +6474,124 @@
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="40" t="s">
+      <c r="A65" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="44" t="s">
+      <c r="A66" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C66" s="44" t="s">
+      <c r="C66" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D66" s="44" t="s">
+      <c r="D66" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="43">
+      <c r="B67" s="18">
         <f>SUMPRODUCT(B57:B62/100, G57:G62*J57:J62)/SQRT((1-0.3)*SUMPRODUCT((B57:B62/100)^2, J57:J62^2) + 0.3*(SUMPRODUCT(B57:B62/100, J57:J62))^2)</f>
         <v>1.5124597854568231</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="18">
         <f>SUMPRODUCT(B57:B62/100, I57:I62)</f>
         <v>11.243639367020569</v>
       </c>
-      <c r="D67" s="43" t="s">
+      <c r="D67" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="43">
+      <c r="B68" s="18">
         <f>SUMPRODUCT(C57:C62/100, G57:G62*J57:J62)/SQRT((1-0.3)*SUMPRODUCT((C57:C62/100)^2, J57:J62^2) + 0.3*(SUMPRODUCT(C57:C62/100, J57:J62))^2)</f>
         <v>1.5182052584218135</v>
       </c>
-      <c r="C68" s="43">
+      <c r="C68" s="18">
         <f>SUMPRODUCT(C57:C62/100, I57:I62)</f>
         <v>13.342698970331796</v>
       </c>
-      <c r="D68" s="43" t="s">
+      <c r="D68" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="43">
+      <c r="B69" s="18">
         <f>SUMPRODUCT(D57:D62/100, G57:G62*J57:J62)/SQRT((1-0.3)*SUMPRODUCT((D57:D62/100)^2, J57:J62^2) + 0.3*(SUMPRODUCT(D57:D62/100, J57:J62))^2)</f>
         <v>1.5747753214508959</v>
       </c>
-      <c r="C69" s="43">
+      <c r="C69" s="18">
         <f>SUMPRODUCT(D57:D62/100, I57:I62)</f>
         <v>11.394288623718149</v>
       </c>
-      <c r="D69" s="43" t="s">
+      <c r="D69" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="43">
+      <c r="B70" s="18">
         <f>SUMPRODUCT(E57:E62/100, G57:G62*J57:J62)/SQRT((1-0.3)*SUMPRODUCT((E57:E62/100)^2, J57:J62^2) + 0.3*(SUMPRODUCT(E57:E62/100, J57:J62))^2)</f>
         <v>1.5771584028225116</v>
       </c>
-      <c r="C70" s="43">
+      <c r="C70" s="18">
         <f>SUMPRODUCT(E57:E62/100, I57:I62)</f>
         <v>13.332011646824775</v>
       </c>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B71" s="43">
+      <c r="B71" s="18">
         <f>SUMPRODUCT(F57:F62/100, G57:G62*J57:J62)/SQRT((1-0.3)*SUMPRODUCT((F57:F62/100)^2, J57:J62^2) + 0.3*(SUMPRODUCT(F57:F62/100, J57:J62))^2)</f>
         <v>1.5496067286629067</v>
       </c>
-      <c r="C71" s="43">
+      <c r="C71" s="18">
         <f>SUMPRODUCT(F57:F62/100, I57:I62)</f>
         <v>15.784782840550363</v>
       </c>
-      <c r="D71" s="43" t="s">
+      <c r="D71" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -7047,124 +7305,124 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A93" s="40" t="s">
+      <c r="A93" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A94" s="44" t="s">
+      <c r="A94" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B94" s="44" t="s">
+      <c r="B94" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C94" s="44" t="s">
+      <c r="C94" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D94" s="44" t="s">
+      <c r="D94" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A95" s="43" t="s">
+      <c r="A95" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B95" s="43">
+      <c r="B95" s="18">
         <f>SUMPRODUCT(B76:B90/100, G76:G90*J76:J90)/SQRT((1-0.3)*SUMPRODUCT((B76:B90/100)^2, J76:J90^2) + 0.3*(SUMPRODUCT(B76:B90/100, J76:J90))^2)</f>
         <v>2.4474737579274644</v>
       </c>
-      <c r="C95" s="43">
+      <c r="C95" s="18">
         <f>SUMPRODUCT(B76:B90/100, I76:I90)</f>
         <v>7.0545371023719934</v>
       </c>
-      <c r="D95" s="43" t="s">
+      <c r="D95" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A96" s="43" t="s">
+      <c r="A96" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B96" s="43">
+      <c r="B96" s="18">
         <f>SUMPRODUCT(C76:C90/100, G76:G90*J76:J90)/SQRT((1-0.3)*SUMPRODUCT((C76:C90/100)^2, J76:J90^2) + 0.3*(SUMPRODUCT(C76:C90/100, J76:J90))^2)</f>
         <v>3.1125473673456909</v>
       </c>
-      <c r="C96" s="43">
+      <c r="C96" s="18">
         <f>SUMPRODUCT(C76:C90/100, I76:I90)</f>
         <v>9.4981567898780916</v>
       </c>
-      <c r="D96" s="43" t="s">
+      <c r="D96" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A97" s="43" t="s">
+      <c r="A97" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="43">
+      <c r="B97" s="18">
         <f>SUMPRODUCT(D76:D90/100, G76:G90*J76:J90)/SQRT((1-0.3)*SUMPRODUCT((D76:D90/100)^2, J76:J90^2) + 0.3*(SUMPRODUCT(D76:D90/100, J76:J90))^2)</f>
         <v>2.9235927252597431</v>
       </c>
-      <c r="C97" s="43">
+      <c r="C97" s="18">
         <f>SUMPRODUCT(D76:D90/100, I76:I90)</f>
         <v>8.7308663306001844</v>
       </c>
-      <c r="D97" s="43" t="s">
+      <c r="D97" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A98" s="43" t="s">
+      <c r="A98" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B98" s="43">
+      <c r="B98" s="18">
         <f>SUMPRODUCT(E76:E90/100, G76:G90*J76:J90)/SQRT((1-0.3)*SUMPRODUCT((E76:E90/100)^2, J76:J90^2) + 0.3*(SUMPRODUCT(E76:E90/100, J76:J90))^2)</f>
         <v>3.7706073833403297</v>
       </c>
-      <c r="C98" s="43">
+      <c r="C98" s="18">
         <f>SUMPRODUCT(E76:E90/100, I76:I90)</f>
         <v>11.143455006562668</v>
       </c>
-      <c r="D98" s="43" t="s">
+      <c r="D98" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A99" s="43" t="s">
+      <c r="A99" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B99" s="43">
+      <c r="B99" s="18">
         <f>SUMPRODUCT(F76:F90/100, G76:G90*J76:J90)/SQRT((1-0.3)*SUMPRODUCT((F76:F90/100)^2, J76:J90^2) + 0.3*(SUMPRODUCT(F76:F90/100, J76:J90))^2)</f>
         <v>4.3248583399817644</v>
       </c>
-      <c r="C99" s="43">
+      <c r="C99" s="18">
         <f>SUMPRODUCT(F76:F90/100, I76:I90)</f>
         <v>13.227782298440266</v>
       </c>
-      <c r="D99" s="43" t="s">
+      <c r="D99" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="36" t="s">
+      <c r="A102" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="18"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="21"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
@@ -7332,124 +7590,124 @@
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A108" s="40" t="s">
+      <c r="A108" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A109" s="44" t="s">
+      <c r="A109" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B109" s="44" t="s">
+      <c r="B109" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C109" s="44" t="s">
+      <c r="C109" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D109" s="44" t="s">
+      <c r="D109" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A110" s="43" t="s">
+      <c r="A110" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B110" s="43">
+      <c r="B110" s="18">
         <f>SUMPRODUCT(B104:B105/100, G104:G105*J104:J105)/SQRT((1-0.3)*SUMPRODUCT((B104:B105/100)^2, J104:J105^2) + 0.3*(SUMPRODUCT(B104:B105/100, J104:J105))^2)</f>
         <v>3.9015482704863254</v>
       </c>
-      <c r="C110" s="43">
+      <c r="C110" s="18">
         <f>SUMPRODUCT(B104:B105/100, I104:I105)</f>
         <v>15.280886933501581</v>
       </c>
-      <c r="D110" s="43" t="s">
+      <c r="D110" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A111" s="43" t="s">
+      <c r="A111" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="43">
+      <c r="B111" s="18">
         <f>SUMPRODUCT(C104:C105/100, G104:G105*J104:J105)/SQRT((1-0.3)*SUMPRODUCT((C104:C105/100)^2, J104:J105^2) + 0.3*(SUMPRODUCT(C104:C105/100, J104:J105))^2)</f>
         <v>4.8185384498558692</v>
       </c>
-      <c r="C111" s="43">
+      <c r="C111" s="18">
         <f>SUMPRODUCT(C104:C105/100, I104:I105)</f>
         <v>14.086323627945101</v>
       </c>
-      <c r="D111" s="43" t="s">
+      <c r="D111" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A112" s="43" t="s">
+      <c r="A112" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B112" s="43">
+      <c r="B112" s="18">
         <f>SUMPRODUCT(D104:D105/100, G104:G105*J104:J105)/SQRT((1-0.3)*SUMPRODUCT((D104:D105/100)^2, J104:J105^2) + 0.3*(SUMPRODUCT(D104:D105/100, J104:J105))^2)</f>
         <v>5.1815002259512157</v>
       </c>
-      <c r="C112" s="43">
+      <c r="C112" s="18">
         <f>SUMPRODUCT(D104:D105/100, I104:I105)</f>
         <v>13.580176499651802</v>
       </c>
-      <c r="D112" s="43" t="s">
+      <c r="D112" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A113" s="43" t="s">
+      <c r="A113" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="43">
+      <c r="B113" s="18">
         <f>SUMPRODUCT(E104:E105/100, G104:G105*J104:J105)/SQRT((1-0.3)*SUMPRODUCT((E104:E105/100)^2, J104:J105^2) + 0.3*(SUMPRODUCT(E104:E105/100, J104:J105))^2)</f>
         <v>4.6275578173732317</v>
       </c>
-      <c r="C113" s="43">
+      <c r="C113" s="18">
         <f>SUMPRODUCT(E104:E105/100, I104:I105)</f>
         <v>14.335892018073096</v>
       </c>
-      <c r="D113" s="43" t="s">
+      <c r="D113" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A114" s="43" t="s">
+      <c r="A114" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B114" s="43">
+      <c r="B114" s="18">
         <f>SUMPRODUCT(F104:F105/100, G104:G105*J104:J105)/SQRT((1-0.3)*SUMPRODUCT((F104:F105/100)^2, J104:J105^2) + 0.3*(SUMPRODUCT(F104:F105/100, J104:J105))^2)</f>
         <v>5.3237959786334459</v>
       </c>
-      <c r="C114" s="43">
+      <c r="C114" s="18">
         <f>SUMPRODUCT(F104:F105/100, I104:I105)</f>
         <v>13.357247432065556</v>
       </c>
-      <c r="D114" s="43" t="s">
+      <c r="D114" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="30" t="s">
+      <c r="A117" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="B117" s="18"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="18"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="18"/>
-      <c r="H117" s="18"/>
-      <c r="I117" s="18"/>
-      <c r="J117" s="18"/>
-      <c r="K117" s="18"/>
-      <c r="L117" s="18"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="21"/>
+      <c r="G117" s="21"/>
+      <c r="H117" s="21"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="21"/>
+      <c r="K117" s="21"/>
+      <c r="L117" s="21"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
@@ -7743,106 +8001,106 @@
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A126" s="40" t="s">
+      <c r="A126" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B126" s="18"/>
-      <c r="C126" s="18"/>
-      <c r="D126" s="18"/>
-      <c r="E126" s="18"/>
-      <c r="F126" s="18"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A127" s="44" t="s">
+      <c r="A127" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B127" s="44" t="s">
+      <c r="B127" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C127" s="44" t="s">
+      <c r="C127" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D127" s="44" t="s">
+      <c r="D127" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A128" s="43" t="s">
+      <c r="A128" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="43">
+      <c r="B128" s="18">
         <f>SUMPRODUCT(B119:B123/100, G119:G123*J119:J123)/SQRT((1-0.3)*SUMPRODUCT((B119:B123/100)^2, J119:J123^2) + 0.3*(SUMPRODUCT(B119:B123/100, J119:J123))^2)</f>
         <v>1.1589386740747079</v>
       </c>
-      <c r="C128" s="43">
+      <c r="C128" s="18">
         <f>SUMPRODUCT(B119:B123/100, I119:I123)</f>
         <v>15.62685164341187</v>
       </c>
-      <c r="D128" s="43" t="s">
+      <c r="D128" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="43" t="s">
+      <c r="A129" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="43">
+      <c r="B129" s="18">
         <f>SUMPRODUCT(C119:C123/100, G119:G123*J119:J123)/SQRT((1-0.3)*SUMPRODUCT((C119:C123/100)^2, J119:J123^2) + 0.3*(SUMPRODUCT(C119:C123/100, J119:J123))^2)</f>
         <v>1.3055274186244001</v>
       </c>
-      <c r="C129" s="43">
+      <c r="C129" s="18">
         <f>SUMPRODUCT(C119:C123/100, I119:I123)</f>
         <v>14.64711773920463</v>
       </c>
-      <c r="D129" s="43" t="s">
+      <c r="D129" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="43" t="s">
+      <c r="A130" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B130" s="43">
+      <c r="B130" s="18">
         <f>SUMPRODUCT(D119:D123/100, G119:G123*J119:J123)/SQRT((1-0.3)*SUMPRODUCT((D119:D123/100)^2, J119:J123^2) + 0.3*(SUMPRODUCT(D119:D123/100, J119:J123))^2)</f>
         <v>1.2022566056977217</v>
       </c>
-      <c r="C130" s="43">
+      <c r="C130" s="18">
         <f>SUMPRODUCT(D119:D123/100, I119:I123)</f>
         <v>15.706796080601684</v>
       </c>
-      <c r="D130" s="43" t="s">
+      <c r="D130" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="43" t="s">
+      <c r="A131" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B131" s="43">
+      <c r="B131" s="18">
         <f>SUMPRODUCT(E119:E123/100, G119:G123*J119:J123)/SQRT((1-0.3)*SUMPRODUCT((E119:E123/100)^2, J119:J123^2) + 0.3*(SUMPRODUCT(E119:E123/100, J119:J123))^2)</f>
         <v>1.2064074575283454</v>
       </c>
-      <c r="C131" s="43">
+      <c r="C131" s="18">
         <f>SUMPRODUCT(E119:E123/100, I119:I123)</f>
         <v>15.409903379891482</v>
       </c>
-      <c r="D131" s="43" t="s">
+      <c r="D131" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="43" t="s">
+      <c r="A132" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B132" s="43">
+      <c r="B132" s="18">
         <f>SUMPRODUCT(F119:F123/100, G119:G123*J119:J123)/SQRT((1-0.3)*SUMPRODUCT((F119:F123/100)^2, J119:J123^2) + 0.3*(SUMPRODUCT(F119:F123/100, J119:J123))^2)</f>
         <v>1.384094874315436</v>
       </c>
-      <c r="C132" s="43">
+      <c r="C132" s="18">
         <f>SUMPRODUCT(F119:F123/100, I119:I123)</f>
         <v>15.011041993026213</v>
       </c>
-      <c r="D132" s="43" t="s">
+      <c r="D132" s="18" t="s">
         <v>183</v>
       </c>
     </row>
@@ -7874,7 +8132,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7884,52 +8142,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -8297,28 +8555,28 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="17" t="s">
         <v>196</v>
       </c>
     </row>
@@ -8338,7 +8596,7 @@
         <f>SUMPRODUCT(G6:G12/100, D6:D12)</f>
         <v>118.53442896649068</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="18" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8358,7 +8616,7 @@
         <f>SUMPRODUCT(H6:H12/100, D6:D12)</f>
         <v>89.129789946105305</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="18" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8378,7 +8636,7 @@
         <f>SUMPRODUCT(I6:I12/100, D6:D12)</f>
         <v>120.56348986480511</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="18" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8398,7 +8656,7 @@
         <f>SUMPRODUCT(J6:J12/100, D6:D12)</f>
         <v>99.100577837286963</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="18" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8418,7 +8676,7 @@
         <f>SUMPRODUCT(K6:K12/100, D6:D12)</f>
         <v>105.51559815172395</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="18" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8437,8 +8695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:J66"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8450,32 +8708,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -8547,32 +8805,32 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -8864,32 +9122,32 @@
       <c r="J26" s="10"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
@@ -9170,14 +9428,14 @@
       <c r="H39" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
@@ -9279,283 +9537,294 @@
       <c r="C53" s="9"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="29"/>
-      <c r="J57" s="29"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="41"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="26"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" s="21" t="s">
+      <c r="A72" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" s="26"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" s="21" t="s">
+      <c r="A75" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="21" t="s">
+      <c r="A76" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A72:J72"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A63:J63"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="A67:J67"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A71:J71"/>
     <mergeCell ref="A77:J77"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A73:J73"/>
@@ -9572,17 +9841,6 @@
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A72:J72"/>
-    <mergeCell ref="A68:J68"/>
-    <mergeCell ref="A63:J63"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A58:J58"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A71:J71"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>